<commit_message>
Update return logic and fix code flow
</commit_message>
<xml_diff>
--- a/registrations.xlsx
+++ b/registrations.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,6 +457,93 @@
           <t>College/Company</t>
         </is>
       </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Blood Donation</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Blood Group</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Webinar Interest</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Webinar Date</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Registered At</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Good Tester</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>9111111111</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>good@test.local</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>IT Professional</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Good College</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>A+</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>2025-12-24 16:58:59</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>